<commit_message>
expanded restricted brandsin restriction list
</commit_message>
<xml_diff>
--- a/restriction_list.xlsx
+++ b/restriction_list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10917"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Python for analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paskag/Desktop/WORK EN Trade/automation_of_analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ABA16F8-D498-4755-882B-EF4228F0F75D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{152B62C3-4A96-0640-8439-6B98602772DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="15120" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$A$60</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="133">
   <si>
     <t>amika</t>
   </si>
@@ -427,6 +427,15 @@
   </si>
   <si>
     <t>revitalash</t>
+  </si>
+  <si>
+    <t>angel</t>
+  </si>
+  <si>
+    <t>tresor</t>
+  </si>
+  <si>
+    <t>idole</t>
   </si>
 </sst>
 </file>
@@ -437,7 +446,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -445,7 +454,7 @@
       <b/>
       <sz val="10"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -453,7 +462,7 @@
       <b/>
       <sz val="9"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -461,7 +470,7 @@
       <b/>
       <sz val="9"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -526,160 +535,20 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="29">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="15">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1106,16 +975,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A130"/>
+  <dimension ref="A1:A134"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A122" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B130" sqref="B130"/>
+      <pane ySplit="1" topLeftCell="A113" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A127" sqref="A127:A133"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.625" customWidth="1"/>
+    <col min="1" max="1" width="19.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
@@ -1144,7 +1013,7 @@
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="2" t="s">
         <v>115</v>
       </c>
     </row>
@@ -1214,7 +1083,7 @@
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20" s="6" t="s">
+      <c r="A20" s="2" t="s">
         <v>125</v>
       </c>
     </row>
@@ -1369,7 +1238,7 @@
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A51" s="6" t="s">
+      <c r="A51" s="2" t="s">
         <v>126</v>
       </c>
     </row>
@@ -1384,7 +1253,7 @@
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A54" s="6" t="s">
+      <c r="A54" s="2" t="s">
         <v>116</v>
       </c>
     </row>
@@ -1404,17 +1273,17 @@
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A58" s="6" t="s">
+      <c r="A58" s="2" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A59" s="6" t="s">
+      <c r="A59" s="2" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A60" s="6" t="s">
+      <c r="A60" s="2" t="s">
         <v>117</v>
       </c>
     </row>
@@ -1424,7 +1293,7 @@
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A62" s="6" t="s">
+      <c r="A62" s="2" t="s">
         <v>120</v>
       </c>
     </row>
@@ -1529,7 +1398,7 @@
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A83" s="7" t="s">
+      <c r="A83" s="5" t="s">
         <v>127</v>
       </c>
     </row>
@@ -1554,7 +1423,7 @@
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A88" s="6" t="s">
+      <c r="A88" s="2" t="s">
         <v>121</v>
       </c>
     </row>
@@ -1594,7 +1463,7 @@
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A96" s="6" t="s">
+      <c r="A96" s="2" t="s">
         <v>128</v>
       </c>
     </row>
@@ -1654,7 +1523,7 @@
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A108" s="7" t="s">
+      <c r="A108" s="5" t="s">
         <v>129</v>
       </c>
     </row>
@@ -1704,12 +1573,12 @@
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A118" s="6" t="s">
+      <c r="A118" s="2" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A119" s="6" t="s">
+      <c r="A119" s="2" t="s">
         <v>123</v>
       </c>
     </row>
@@ -1749,7 +1618,7 @@
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A127" s="5" t="s">
+      <c r="A127" s="2" t="s">
         <v>124</v>
       </c>
     </row>
@@ -1767,6 +1636,24 @@
       <c r="A130" s="2" t="s">
         <v>105</v>
       </c>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A131" s="7" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A132" s="7" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A133" s="7" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A134" s="6"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:A60" xr:uid="{00000000-0001-0000-0000-000000000000}">
@@ -1775,27 +1662,27 @@
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="A1:A108 A110:A127 A129 A131:A1048576">
-    <cfRule type="duplicateValues" dxfId="28" priority="9"/>
-    <cfRule type="duplicateValues" dxfId="27" priority="10"/>
-    <cfRule type="duplicateValues" dxfId="26" priority="11"/>
-    <cfRule type="duplicateValues" dxfId="25" priority="12"/>
-    <cfRule type="duplicateValues" dxfId="24" priority="13"/>
-    <cfRule type="duplicateValues" dxfId="23" priority="14"/>
-    <cfRule type="duplicateValues" dxfId="22" priority="15"/>
+    <cfRule type="duplicateValues" dxfId="14" priority="15"/>
+    <cfRule type="duplicateValues" dxfId="13" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="12" priority="14"/>
+    <cfRule type="duplicateValues" dxfId="11" priority="13"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="12"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A127 A129 A131:A1048576">
-    <cfRule type="duplicateValues" dxfId="21" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:A1048576">
+    <cfRule type="duplicateValues" dxfId="6" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A109">
-    <cfRule type="duplicateValues" dxfId="20" priority="3"/>
-    <cfRule type="duplicateValues" dxfId="19" priority="4"/>
-    <cfRule type="duplicateValues" dxfId="18" priority="5"/>
-    <cfRule type="duplicateValues" dxfId="17" priority="6"/>
-    <cfRule type="duplicateValues" dxfId="16" priority="7"/>
-    <cfRule type="duplicateValues" dxfId="15" priority="8"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="8"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added brands in hebrew
</commit_message>
<xml_diff>
--- a/restriction_list.xlsx
+++ b/restriction_list.xlsx
@@ -1,24 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paskag/Desktop/WORK_EN_Trade/automation_of_analysis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Python for analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E76B877-4304-EB4C-8864-93A3F4C616AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCC87360-A9FE-431D-967B-F04A395CDF38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="15120" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$A$60</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$A$156</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="185">
   <si>
     <t>amika</t>
   </si>
@@ -360,9 +360,6 @@
     <t>brand</t>
   </si>
   <si>
-    <t>bvlgari</t>
-  </si>
-  <si>
     <t>thierry mugler</t>
   </si>
   <si>
@@ -439,6 +436,162 @@
   </si>
   <si>
     <t>burerry</t>
+  </si>
+  <si>
+    <t>טסטר</t>
+  </si>
+  <si>
+    <t>אולפלקס</t>
+  </si>
+  <si>
+    <t>אזארו</t>
+  </si>
+  <si>
+    <t>אלי סאאב</t>
+  </si>
+  <si>
+    <t>אסנטריק מולקולה</t>
+  </si>
+  <si>
+    <t>אסקדה</t>
+  </si>
+  <si>
+    <t>בוס</t>
+  </si>
+  <si>
+    <t>הוגו בוס</t>
+  </si>
+  <si>
+    <t>ברברי</t>
+  </si>
+  <si>
+    <t>ג'ימי צ'ו</t>
+  </si>
+  <si>
+    <t>דוידוף</t>
+  </si>
+  <si>
+    <t>דיזל</t>
+  </si>
+  <si>
+    <t>ויקטור אנד רולף</t>
+  </si>
+  <si>
+    <t>לליק</t>
+  </si>
+  <si>
+    <t>לנוין</t>
+  </si>
+  <si>
+    <t>סוספירו קסרג'וף</t>
+  </si>
+  <si>
+    <t>קסרג'וף</t>
+  </si>
+  <si>
+    <t>קואץ'</t>
+  </si>
+  <si>
+    <t>קלין</t>
+  </si>
+  <si>
+    <t>קסרג'וף קאסמורטי</t>
+  </si>
+  <si>
+    <t>קריד</t>
+  </si>
+  <si>
+    <t>רוברטו קוואלי</t>
+  </si>
+  <si>
+    <t>רושאס</t>
+  </si>
+  <si>
+    <t>אלפאפארף </t>
+  </si>
+  <si>
+    <t>אמיקה </t>
+  </si>
+  <si>
+    <t>אמואג'</t>
+  </si>
+  <si>
+    <t>אריאנה גרנדה</t>
+  </si>
+  <si>
+    <t>אריאנה</t>
+  </si>
+  <si>
+    <t>אוון</t>
+  </si>
+  <si>
+    <t xml:space="preserve">באבור </t>
+  </si>
+  <si>
+    <t>בוס הוגו</t>
+  </si>
+  <si>
+    <t>בוס הוגו בוס</t>
+  </si>
+  <si>
+    <t>קלווין </t>
+  </si>
+  <si>
+    <t>קלווין קליין</t>
+  </si>
+  <si>
+    <t>קלרינס </t>
+  </si>
+  <si>
+    <t>דנהיל</t>
+  </si>
+  <si>
+    <t>אלמיס </t>
+  </si>
+  <si>
+    <t>אליזבת ארדן</t>
+  </si>
+  <si>
+    <t>גרלן</t>
+  </si>
+  <si>
+    <t>הוגו</t>
+  </si>
+  <si>
+    <t>ג'וסי קוטור</t>
+  </si>
+  <si>
+    <t>ג'וסי</t>
+  </si>
+  <si>
+    <t>לוריאל פרופשיונל</t>
+  </si>
+  <si>
+    <t>לוריאל</t>
+  </si>
+  <si>
+    <t>לקוסט </t>
+  </si>
+  <si>
+    <t>לנקום</t>
+  </si>
+  <si>
+    <t>ראלף לורן</t>
+  </si>
+  <si>
+    <t>לורן</t>
+  </si>
+  <si>
+    <t>מונט בלאן</t>
+  </si>
+  <si>
+    <t>מונטל </t>
+  </si>
+  <si>
+    <t>מוגלר</t>
+  </si>
+  <si>
+    <t>נוקס </t>
   </si>
 </sst>
 </file>
@@ -449,7 +602,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -457,7 +610,7 @@
       <b/>
       <sz val="10"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -465,7 +618,7 @@
       <b/>
       <sz val="9"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -473,7 +626,7 @@
       <b/>
       <sz val="9"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -972,16 +1125,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A134"/>
+  <dimension ref="A1:A185"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A125" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D124" sqref="D124"/>
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B162" sqref="B162"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.6640625" customWidth="1"/>
+    <col min="1" max="1" width="19.625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
@@ -1006,17 +1159,17 @@
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.2">
@@ -1066,127 +1219,127 @@
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>107</v>
+        <v>6</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>6</v>
+        <v>59</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>59</v>
+        <v>7</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>7</v>
+        <v>124</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>125</v>
+        <v>80</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>84</v>
+        <v>60</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>60</v>
+        <v>8</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>10</v>
+        <v>74</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>74</v>
+        <v>11</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>11</v>
+        <v>85</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
-        <v>85</v>
+        <v>12</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>14</v>
+        <v>71</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>71</v>
+        <v>15</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>15</v>
+        <v>86</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
-        <v>87</v>
+        <v>16</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.2">
@@ -1196,392 +1349,392 @@
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
-        <v>19</v>
+        <v>110</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
-        <v>111</v>
+        <v>20</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
-        <v>20</v>
+        <v>88</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
-        <v>72</v>
+        <v>21</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
-        <v>21</v>
+        <v>61</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
-        <v>61</v>
+        <v>23</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
-        <v>23</v>
+        <v>131</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
-        <v>132</v>
+        <v>22</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
-        <v>22</v>
+        <v>125</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
-        <v>126</v>
+        <v>67</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
-        <v>67</v>
+        <v>25</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
-        <v>25</v>
+        <v>115</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
-        <v>116</v>
+        <v>26</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
-        <v>26</v>
+        <v>73</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
-        <v>73</v>
+        <v>27</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
-        <v>27</v>
+        <v>118</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
-        <v>117</v>
+        <v>28</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
-        <v>28</v>
+        <v>119</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
-        <v>120</v>
+        <v>29</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
-        <v>30</v>
+        <v>89</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
-        <v>89</v>
+        <v>31</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
-        <v>31</v>
+        <v>76</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A70" s="5" t="s">
-        <v>127</v>
+      <c r="A70" s="2" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
-        <v>78</v>
+        <v>112</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A74" s="2" t="s">
-        <v>79</v>
+        <v>32</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
-        <v>113</v>
+        <v>33</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A76" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A77" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A78" s="2" t="s">
-        <v>34</v>
+        <v>93</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
-        <v>35</v>
+        <v>99</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A80" s="2" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A81" s="2" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A82" s="2" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A83" s="2" t="s">
-        <v>94</v>
+        <v>75</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A84" s="2" t="s">
-        <v>90</v>
+        <v>36</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A85" s="2" t="s">
-        <v>75</v>
+      <c r="A85" s="5" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A86" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A87" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A88" s="2" t="s">
-        <v>38</v>
+        <v>111</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A89" s="2" t="s">
-        <v>112</v>
+        <v>91</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A90" s="2" t="s">
-        <v>91</v>
+        <v>120</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A91" s="2" t="s">
-        <v>121</v>
+        <v>39</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A92" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A93" s="2" t="s">
-        <v>40</v>
+        <v>63</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A94" s="2" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A95" s="2" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A96" s="2" t="s">
-        <v>64</v>
+        <v>41</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A97" s="2" t="s">
-        <v>41</v>
+        <v>108</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A98" s="2" t="s">
-        <v>109</v>
+        <v>127</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A99" s="2" t="s">
-        <v>128</v>
+        <v>66</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A100" s="2" t="s">
-        <v>66</v>
+        <v>42</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A101" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A102" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A103" s="2" t="s">
-        <v>44</v>
+        <v>100</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A104" s="2" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A105" s="2" t="s">
-        <v>96</v>
+        <v>46</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A106" s="2" t="s">
-        <v>46</v>
+        <v>92</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A107" s="2" t="s">
-        <v>92</v>
+        <v>65</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A108" s="2" t="s">
-        <v>65</v>
+        <v>45</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A109" s="2" t="s">
-        <v>45</v>
+        <v>69</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A110" s="2" t="s">
-        <v>69</v>
+        <v>128</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A111" s="5" t="s">
-        <v>129</v>
+      <c r="A111" s="2" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A112" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A113" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A114" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A115" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A116" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A117" s="2" t="s">
-        <v>52</v>
+        <v>102</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A118" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A119" s="2" t="s">
-        <v>101</v>
+        <v>53</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A120" s="2" t="s">
-        <v>53</v>
+        <v>121</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.2">
@@ -1591,96 +1744,351 @@
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A122" s="2" t="s">
-        <v>123</v>
+        <v>107</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A123" s="2" t="s">
-        <v>108</v>
+        <v>54</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A124" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A125" s="2" t="s">
-        <v>55</v>
+      <c r="A125" s="4" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A126" s="4" t="s">
-        <v>131</v>
+      <c r="A126" s="2" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A127" s="2" t="s">
-        <v>56</v>
+        <v>103</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A128" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A129" s="2" t="s">
-        <v>104</v>
+        <v>70</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A130" s="2" t="s">
-        <v>70</v>
+        <v>123</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A131" s="2" t="s">
-        <v>124</v>
+        <v>57</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A132" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A133" s="2" t="s">
-        <v>58</v>
+        <v>105</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A134" s="2" t="s">
-        <v>105</v>
+        <v>161</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A135" s="2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A136" s="2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A137" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A138" s="2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A139" s="2" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A140" s="2" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A141" s="2" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A142" s="2" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A143" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A144" s="2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A145" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A146" s="2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A147" s="2" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A148" s="2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="149" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A149" s="2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="150" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A150" s="2" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="151" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A151" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A152" s="2" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="153" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A153" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="154" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A154" s="2" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="155" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A155" s="2" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="156" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A156" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="157" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A157" s="2" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="158" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A158" s="2" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="159" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A159" s="2" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="160" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A160" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="161" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A161" s="2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A162" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="163" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A163" s="2" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="164" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A164" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="165" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A165" s="2" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="166" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A166" s="2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="167" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A167" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="168" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A168" s="2" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="169" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A169" s="2" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="170" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A170" s="2" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="171" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A171" s="2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="172" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A172" s="2" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="173" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A173" s="2" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="174" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A174" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="175" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A175" s="2" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="176" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A176" s="2" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="177" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A177" s="2" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="178" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A178" s="2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="179" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A179" s="2" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="180" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A180" s="2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="181" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A181" s="2" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="182" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A182" s="2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="183" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A183" s="2" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="184" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A184" s="2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="185" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A185" s="2" t="s">
+        <v>155</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:A60" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A134">
-      <sortCondition ref="A1:A134"/>
+  <autoFilter ref="A1:A156" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A186">
+      <sortCondition ref="A1:A156"/>
     </sortState>
   </autoFilter>
-  <conditionalFormatting sqref="A1:A108 A110:A127 A129 A131:A1048576">
-    <cfRule type="duplicateValues" dxfId="14" priority="15"/>
-    <cfRule type="duplicateValues" dxfId="13" priority="9"/>
-    <cfRule type="duplicateValues" dxfId="12" priority="14"/>
-    <cfRule type="duplicateValues" dxfId="11" priority="13"/>
-    <cfRule type="duplicateValues" dxfId="10" priority="12"/>
-    <cfRule type="duplicateValues" dxfId="9" priority="11"/>
-    <cfRule type="duplicateValues" dxfId="8" priority="10"/>
+  <conditionalFormatting sqref="A1:A107 A128 A109:A126 A130:A1048576">
+    <cfRule type="duplicateValues" dxfId="14" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="13" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="12" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="11" priority="12"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="13"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="14"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="15"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:A127 A129 A131:A1048576">
+  <conditionalFormatting sqref="A128 A1:A126 A130:A1048576">
     <cfRule type="duplicateValues" dxfId="7" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A1048576">
     <cfRule type="duplicateValues" dxfId="6" priority="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A109">
-    <cfRule type="duplicateValues" dxfId="5" priority="7"/>
-    <cfRule type="duplicateValues" dxfId="4" priority="6"/>
+  <conditionalFormatting sqref="A108">
+    <cfRule type="duplicateValues" dxfId="5" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="4"/>
     <cfRule type="duplicateValues" dxfId="3" priority="5"/>
-    <cfRule type="duplicateValues" dxfId="2" priority="4"/>
-    <cfRule type="duplicateValues" dxfId="1" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="7"/>
     <cfRule type="duplicateValues" dxfId="0" priority="8"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added some new brands
</commit_message>
<xml_diff>
--- a/restriction_list.xlsx
+++ b/restriction_list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Python for analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{482C06A3-B364-4A31-906E-66B0EADDAD21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A535AF89-F8D2-4B77-A701-A68BD491458C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9090" yWindow="1980" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="221">
   <si>
     <t>amika</t>
   </si>
@@ -688,6 +688,18 @@
   </si>
   <si>
     <t>escentricmolecule</t>
+  </si>
+  <si>
+    <t>juliette</t>
+  </si>
+  <si>
+    <t>thierry</t>
+  </si>
+  <si>
+    <t>bioderma</t>
+  </si>
+  <si>
+    <t>l'occittane</t>
   </si>
 </sst>
 </file>
@@ -803,7 +815,17 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="20">
+  <dxfs count="21">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1280,11 +1302,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A217"/>
+  <dimension ref="A1:A221"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H8" sqref="H8"/>
+      <selection pane="bottomLeft" activeCell="C216" sqref="C216"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1349,1070 +1371,1093 @@
     </row>
     <row r="12" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>60</v>
+        <v>219</v>
       </c>
     </row>
     <row r="13" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>94</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>22</v>
+        <v>94</v>
       </c>
     </row>
     <row r="15" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>210</v>
+        <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>5</v>
+        <v>210</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>129</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>215</v>
+        <v>129</v>
       </c>
     </row>
     <row r="20" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>6</v>
+        <v>215</v>
       </c>
     </row>
     <row r="21" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>57</v>
+        <v>6</v>
       </c>
     </row>
     <row r="22" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>7</v>
+        <v>57</v>
       </c>
     </row>
     <row r="23" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>121</v>
+        <v>7</v>
       </c>
     </row>
     <row r="24" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>199</v>
+        <v>121</v>
       </c>
     </row>
     <row r="25" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>78</v>
+        <v>199</v>
       </c>
     </row>
     <row r="26" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="27" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>58</v>
+        <v>82</v>
       </c>
     </row>
     <row r="28" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>8</v>
+        <v>58</v>
       </c>
     </row>
     <row r="29" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="30" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="31" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>72</v>
+        <v>10</v>
       </c>
     </row>
     <row r="32" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>214</v>
+        <v>72</v>
       </c>
     </row>
     <row r="33" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>11</v>
+        <v>214</v>
       </c>
     </row>
     <row r="34" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>181</v>
+        <v>11</v>
       </c>
     </row>
     <row r="35" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>206</v>
+        <v>181</v>
       </c>
     </row>
     <row r="36" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>12</v>
+        <v>206</v>
       </c>
     </row>
     <row r="37" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="38" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>69</v>
+        <v>13</v>
       </c>
     </row>
     <row r="39" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>14</v>
+        <v>69</v>
       </c>
     </row>
     <row r="40" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>83</v>
+        <v>14</v>
       </c>
     </row>
     <row r="41" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>197</v>
+        <v>83</v>
       </c>
     </row>
     <row r="42" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>84</v>
+        <v>197</v>
       </c>
     </row>
     <row r="43" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>15</v>
+        <v>84</v>
       </c>
     </row>
     <row r="44" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="45" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="46" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="47" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>95</v>
+        <v>18</v>
       </c>
     </row>
     <row r="48" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>216</v>
+        <v>95</v>
       </c>
     </row>
     <row r="49" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>107</v>
+        <v>216</v>
       </c>
     </row>
     <row r="50" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="51" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>19</v>
+        <v>106</v>
       </c>
     </row>
     <row r="52" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>85</v>
+        <v>19</v>
       </c>
     </row>
     <row r="53" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>70</v>
+        <v>85</v>
       </c>
     </row>
     <row r="54" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>202</v>
+        <v>70</v>
       </c>
     </row>
     <row r="55" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>59</v>
+        <v>202</v>
       </c>
     </row>
     <row r="56" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
-        <v>21</v>
+        <v>59</v>
       </c>
     </row>
     <row r="57" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
-        <v>128</v>
+        <v>21</v>
       </c>
     </row>
     <row r="58" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>20</v>
+        <v>128</v>
       </c>
     </row>
     <row r="59" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
-        <v>122</v>
+        <v>20</v>
       </c>
     </row>
     <row r="60" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
-        <v>65</v>
+        <v>122</v>
       </c>
     </row>
     <row r="61" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
-        <v>23</v>
+        <v>65</v>
       </c>
     </row>
     <row r="62" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
-        <v>112</v>
+        <v>23</v>
       </c>
     </row>
     <row r="63" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
-        <v>24</v>
+        <v>112</v>
       </c>
     </row>
     <row r="64" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
-        <v>71</v>
+        <v>24</v>
       </c>
     </row>
     <row r="65" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
-        <v>25</v>
+        <v>71</v>
       </c>
     </row>
     <row r="66" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
-        <v>115</v>
+        <v>25</v>
       </c>
     </row>
     <row r="67" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="68" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="69" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
-        <v>26</v>
+        <v>113</v>
       </c>
     </row>
     <row r="70" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
-        <v>116</v>
+        <v>217</v>
       </c>
     </row>
     <row r="71" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="72" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
-        <v>195</v>
+        <v>116</v>
       </c>
     </row>
     <row r="73" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
-        <v>207</v>
+        <v>27</v>
       </c>
     </row>
     <row r="74" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
-        <v>28</v>
+        <v>195</v>
       </c>
     </row>
     <row r="75" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
-        <v>86</v>
+        <v>207</v>
       </c>
     </row>
     <row r="76" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="77" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
-        <v>74</v>
+        <v>86</v>
       </c>
     </row>
     <row r="78" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
-        <v>75</v>
+        <v>29</v>
       </c>
     </row>
     <row r="79" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="80" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="81" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
-        <v>109</v>
+        <v>76</v>
       </c>
     </row>
     <row r="82" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
-        <v>30</v>
+        <v>77</v>
       </c>
     </row>
     <row r="83" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
-        <v>31</v>
+        <v>109</v>
       </c>
     </row>
     <row r="84" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="85" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="86" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
-        <v>90</v>
+        <v>32</v>
       </c>
     </row>
     <row r="87" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
-        <v>96</v>
+        <v>33</v>
       </c>
     </row>
     <row r="88" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="89" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
     </row>
     <row r="90" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
     </row>
     <row r="91" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
-        <v>73</v>
+        <v>91</v>
       </c>
     </row>
     <row r="92" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
-        <v>198</v>
+        <v>87</v>
       </c>
     </row>
     <row r="93" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
-        <v>34</v>
+        <v>73</v>
       </c>
     </row>
     <row r="94" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A94" s="4" t="s">
-        <v>123</v>
+      <c r="A94" s="1" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="95" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
-        <v>204</v>
+        <v>34</v>
       </c>
     </row>
     <row r="96" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A96" s="1" t="s">
-        <v>35</v>
+      <c r="A96" s="4" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="97" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
     </row>
     <row r="98" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
-        <v>36</v>
+        <v>220</v>
       </c>
     </row>
     <row r="99" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
-        <v>108</v>
+        <v>35</v>
       </c>
     </row>
     <row r="100" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
     </row>
     <row r="101" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
-        <v>205</v>
+        <v>36</v>
       </c>
     </row>
     <row r="102" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
-        <v>212</v>
+        <v>108</v>
       </c>
     </row>
     <row r="103" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
-        <v>88</v>
+        <v>213</v>
       </c>
     </row>
     <row r="104" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
-        <v>117</v>
+        <v>205</v>
       </c>
     </row>
     <row r="105" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
-        <v>37</v>
+        <v>212</v>
       </c>
     </row>
     <row r="106" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
-        <v>38</v>
+        <v>88</v>
       </c>
     </row>
     <row r="107" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
-        <v>61</v>
+        <v>117</v>
       </c>
     </row>
     <row r="108" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
-        <v>66</v>
+        <v>37</v>
       </c>
     </row>
     <row r="109" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
-        <v>62</v>
+        <v>38</v>
       </c>
     </row>
     <row r="110" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
-        <v>39</v>
+        <v>61</v>
       </c>
     </row>
     <row r="111" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
-        <v>105</v>
+        <v>66</v>
       </c>
     </row>
     <row r="112" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
-        <v>124</v>
+        <v>62</v>
       </c>
     </row>
     <row r="113" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
-        <v>64</v>
+        <v>39</v>
       </c>
     </row>
     <row r="114" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
-        <v>40</v>
+        <v>105</v>
       </c>
     </row>
     <row r="115" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
-        <v>41</v>
+        <v>124</v>
       </c>
     </row>
     <row r="116" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
-        <v>42</v>
+        <v>64</v>
       </c>
     </row>
     <row r="117" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
-        <v>97</v>
+        <v>40</v>
       </c>
     </row>
     <row r="118" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
-        <v>93</v>
+        <v>41</v>
       </c>
     </row>
     <row r="119" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="120" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
     </row>
     <row r="121" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
-        <v>63</v>
+        <v>93</v>
       </c>
     </row>
     <row r="122" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A122" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="123" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="s">
-        <v>67</v>
+        <v>89</v>
       </c>
     </row>
     <row r="124" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="s">
-        <v>203</v>
+        <v>63</v>
       </c>
     </row>
     <row r="125" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
-        <v>125</v>
+        <v>43</v>
       </c>
     </row>
     <row r="126" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A126" s="1" t="s">
-        <v>45</v>
+        <v>67</v>
       </c>
     </row>
     <row r="127" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A127" s="1" t="s">
-        <v>46</v>
+        <v>203</v>
       </c>
     </row>
     <row r="128" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A128" s="1" t="s">
-        <v>47</v>
+        <v>125</v>
       </c>
     </row>
     <row r="129" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A129" s="1" t="s">
-        <v>196</v>
+        <v>45</v>
       </c>
     </row>
     <row r="130" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A130" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="131" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A131" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="132" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A132" s="1" t="s">
-        <v>50</v>
+        <v>196</v>
       </c>
     </row>
     <row r="133" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A133" s="1" t="s">
-        <v>99</v>
+        <v>48</v>
       </c>
     </row>
     <row r="134" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A134" s="1" t="s">
-        <v>98</v>
+        <v>49</v>
       </c>
     </row>
     <row r="135" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A135" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="136" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A136" s="1" t="s">
-        <v>118</v>
+        <v>99</v>
       </c>
     </row>
     <row r="137" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A137" s="1" t="s">
-        <v>119</v>
+        <v>98</v>
       </c>
     </row>
     <row r="138" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A138" s="1" t="s">
-        <v>104</v>
+        <v>51</v>
       </c>
     </row>
     <row r="139" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A139" s="1" t="s">
-        <v>200</v>
+        <v>118</v>
       </c>
     </row>
     <row r="140" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A140" s="1" t="s">
-        <v>52</v>
+        <v>119</v>
       </c>
     </row>
     <row r="141" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A141" s="1" t="s">
-        <v>53</v>
+        <v>218</v>
       </c>
     </row>
     <row r="142" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A142" s="1" t="s">
-        <v>127</v>
+        <v>104</v>
       </c>
     </row>
     <row r="143" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A143" s="1" t="s">
-        <v>54</v>
+        <v>200</v>
       </c>
     </row>
     <row r="144" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A144" s="1" t="s">
-        <v>100</v>
+        <v>52</v>
       </c>
     </row>
     <row r="145" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A145" s="1" t="s">
-        <v>101</v>
+        <v>53</v>
       </c>
     </row>
     <row r="146" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A146" s="1" t="s">
-        <v>68</v>
+        <v>127</v>
       </c>
     </row>
     <row r="147" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A147" s="1" t="s">
-        <v>120</v>
+        <v>54</v>
       </c>
     </row>
     <row r="148" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A148" s="1" t="s">
-        <v>55</v>
+        <v>100</v>
       </c>
     </row>
     <row r="149" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A149" s="1" t="s">
-        <v>201</v>
+        <v>101</v>
       </c>
     </row>
     <row r="150" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A150" s="1" t="s">
-        <v>211</v>
+        <v>68</v>
       </c>
     </row>
     <row r="151" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A151" s="1" t="s">
-        <v>56</v>
+        <v>120</v>
       </c>
     </row>
     <row r="152" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A152" s="1" t="s">
-        <v>208</v>
+        <v>55</v>
       </c>
     </row>
     <row r="153" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A153" s="1" t="s">
-        <v>102</v>
+        <v>201</v>
       </c>
     </row>
     <row r="154" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A154" s="1" t="s">
-        <v>157</v>
+        <v>211</v>
       </c>
     </row>
     <row r="155" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A155" s="1" t="s">
-        <v>131</v>
+        <v>56</v>
       </c>
     </row>
     <row r="156" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A156" s="1" t="s">
-        <v>189</v>
+        <v>208</v>
       </c>
     </row>
     <row r="157" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A157" s="1" t="s">
-        <v>132</v>
+        <v>102</v>
       </c>
     </row>
     <row r="158" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A158" s="1" t="s">
-        <v>133</v>
+        <v>157</v>
       </c>
     </row>
     <row r="159" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A159" s="1" t="s">
-        <v>166</v>
+        <v>131</v>
       </c>
     </row>
     <row r="160" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A160" s="1" t="s">
-        <v>165</v>
+        <v>189</v>
       </c>
     </row>
     <row r="161" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A161" s="1" t="s">
-        <v>152</v>
+        <v>132</v>
       </c>
     </row>
     <row r="162" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A162" s="1" t="s">
-        <v>154</v>
+        <v>133</v>
       </c>
     </row>
     <row r="163" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A163" s="1" t="s">
-        <v>153</v>
+        <v>166</v>
       </c>
     </row>
     <row r="164" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A164" s="1" t="s">
-        <v>180</v>
+        <v>165</v>
       </c>
     </row>
     <row r="165" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A165" s="1" t="s">
-        <v>134</v>
+        <v>152</v>
       </c>
     </row>
     <row r="166" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A166" s="1" t="s">
-        <v>135</v>
+        <v>154</v>
       </c>
     </row>
     <row r="167" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A167" s="1" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="168" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A168" s="1" t="s">
-        <v>155</v>
+        <v>180</v>
       </c>
     </row>
     <row r="169" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A169" s="1" t="s">
-        <v>158</v>
+        <v>134</v>
       </c>
     </row>
     <row r="170" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A170" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="171" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A171" s="1" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="172" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A172" s="1" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
     </row>
     <row r="173" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A173" s="1" t="s">
-        <v>194</v>
+        <v>158</v>
       </c>
     </row>
     <row r="174" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A174" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="175" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A175" s="1" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
     </row>
     <row r="176" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A176" s="1" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
     </row>
     <row r="177" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A177" s="1" t="s">
-        <v>139</v>
+        <v>194</v>
       </c>
     </row>
     <row r="178" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A178" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="179" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A179" s="1" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
     </row>
     <row r="180" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A180" s="1" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="181" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A181" s="1" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
     </row>
     <row r="182" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A182" s="1" t="s">
-        <v>185</v>
+        <v>140</v>
       </c>
     </row>
     <row r="183" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A183" s="1" t="s">
-        <v>141</v>
+        <v>164</v>
       </c>
     </row>
     <row r="184" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A184" s="1" t="s">
-        <v>183</v>
+        <v>167</v>
       </c>
     </row>
     <row r="185" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A185" s="1" t="s">
-        <v>130</v>
+        <v>137</v>
       </c>
     </row>
     <row r="186" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A186" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="187" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A187" s="1" t="s">
-        <v>171</v>
+        <v>141</v>
       </c>
     </row>
     <row r="188" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A188" s="1" t="s">
-        <v>170</v>
+        <v>183</v>
       </c>
     </row>
     <row r="189" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A189" s="1" t="s">
-        <v>175</v>
+        <v>130</v>
       </c>
     </row>
     <row r="190" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A190" s="1" t="s">
-        <v>142</v>
+        <v>187</v>
       </c>
     </row>
     <row r="191" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A191" s="1" t="s">
-        <v>143</v>
+        <v>171</v>
       </c>
     </row>
     <row r="192" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A192" s="1" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="193" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A193" s="1" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
     </row>
     <row r="194" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A194" s="1" t="s">
-        <v>178</v>
+        <v>142</v>
       </c>
     </row>
     <row r="195" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A195" s="1" t="s">
-        <v>176</v>
+        <v>143</v>
       </c>
     </row>
     <row r="196" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A196" s="1" t="s">
-        <v>192</v>
+        <v>173</v>
       </c>
     </row>
     <row r="197" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A197" s="1" t="s">
-        <v>193</v>
+        <v>172</v>
       </c>
     </row>
     <row r="198" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A198" s="1" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="199" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A199" s="1" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
     </row>
     <row r="200" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A200" s="1" t="s">
-        <v>179</v>
+        <v>192</v>
       </c>
     </row>
     <row r="201" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A201" s="1" t="s">
-        <v>144</v>
+        <v>193</v>
       </c>
     </row>
     <row r="202" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A202" s="1" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
     </row>
     <row r="203" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A203" s="1" t="s">
-        <v>146</v>
+        <v>186</v>
       </c>
     </row>
     <row r="204" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A204" s="1" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
     </row>
     <row r="205" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A205" s="1" t="s">
-        <v>161</v>
+        <v>144</v>
       </c>
     </row>
     <row r="206" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A206" s="1" t="s">
-        <v>162</v>
+        <v>184</v>
       </c>
     </row>
     <row r="207" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A207" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="208" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A208" s="1" t="s">
-        <v>163</v>
+        <v>188</v>
       </c>
     </row>
     <row r="209" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A209" s="1" t="s">
-        <v>190</v>
+        <v>161</v>
       </c>
     </row>
     <row r="210" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A210" s="1" t="s">
-        <v>191</v>
+        <v>162</v>
       </c>
     </row>
     <row r="211" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A211" s="1" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
     </row>
     <row r="212" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A212" s="1" t="s">
-        <v>148</v>
+        <v>163</v>
       </c>
     </row>
     <row r="213" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A213" s="1" t="s">
-        <v>149</v>
+        <v>190</v>
       </c>
     </row>
     <row r="214" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A214" s="1" t="s">
-        <v>174</v>
+        <v>191</v>
       </c>
     </row>
     <row r="215" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A215" s="1" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
     </row>
     <row r="216" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A216" s="1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="217" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A217" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="218" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A218" s="1" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="219" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A219" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="220" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A220" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="221" spans="1:1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A221" s="1" t="s">
         <v>182</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:A153" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A217">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A221">
       <sortCondition ref="A1:A153"/>
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="duplicateValues" dxfId="19" priority="4"/>
-    <cfRule type="duplicateValues" dxfId="18" priority="5"/>
-    <cfRule type="duplicateValues" dxfId="17" priority="6"/>
-    <cfRule type="duplicateValues" dxfId="16" priority="66"/>
+    <cfRule type="duplicateValues" dxfId="20" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="19" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="18" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="17" priority="67"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A105">
-    <cfRule type="duplicateValues" dxfId="15" priority="8"/>
-    <cfRule type="duplicateValues" dxfId="14" priority="9"/>
-    <cfRule type="duplicateValues" dxfId="13" priority="10"/>
-    <cfRule type="duplicateValues" dxfId="12" priority="11"/>
-    <cfRule type="duplicateValues" dxfId="11" priority="12"/>
-    <cfRule type="duplicateValues" dxfId="10" priority="13"/>
+    <cfRule type="duplicateValues" dxfId="16" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="15" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="14" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="13" priority="12"/>
+    <cfRule type="duplicateValues" dxfId="12" priority="13"/>
+    <cfRule type="duplicateValues" dxfId="11" priority="14"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A125 A1:A104 A106:A123 A127:A1048576">
-    <cfRule type="duplicateValues" dxfId="9" priority="14"/>
-    <cfRule type="duplicateValues" dxfId="8" priority="15"/>
-    <cfRule type="duplicateValues" dxfId="7" priority="16"/>
-    <cfRule type="duplicateValues" dxfId="6" priority="17"/>
-    <cfRule type="duplicateValues" dxfId="5" priority="18"/>
-    <cfRule type="duplicateValues" dxfId="4" priority="19"/>
-    <cfRule type="duplicateValues" dxfId="3" priority="20"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="15"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="16"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="17"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="18"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="19"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="20"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="21"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A125 A1:A123 A127:A1048576">
-    <cfRule type="duplicateValues" dxfId="2" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A204:A205">
+    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A207:A221">
     <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A207:A217">
+  <conditionalFormatting sqref="A219">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>